<commit_message>
edits to respiration data and calc O:N ratio
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Excretion/20211026_Excretion_raw.xlsx
+++ b/RAnalysis/Data/Excretion/20211026_Excretion_raw.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="0" windowWidth="21864" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="2352" yWindow="0" windowWidth="21864" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Excretion 10-26-21" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
   <si>
     <t>Standard Addition Determination of Ammonia-N Concentration in Seawater Blank</t>
   </si>
@@ -309,6 +309,12 @@
   <si>
     <t>mmol/L/hr</t>
   </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
 </sst>
 </file>
 
@@ -317,7 +323,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -497,10 +503,6 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -544,7 +546,7 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -572,6 +574,10 @@
     <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,7 +653,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -926,7 +931,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1030,7 +1034,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -1093,7 +1096,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -1407,15 +1409,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6982,1040 +6984,1056 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="19.3984375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="17.796875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="5.09765625" style="20" customWidth="1"/>
-    <col min="6" max="7" width="13.59765625" style="17" customWidth="1"/>
-    <col min="8" max="17" width="13.59765625" style="15" customWidth="1"/>
-    <col min="18" max="18" width="5.09765625" style="20" customWidth="1"/>
-    <col min="19" max="19" width="14.19921875" style="15" customWidth="1"/>
-    <col min="20" max="20" width="16.19921875" style="15" customWidth="1"/>
-    <col min="21" max="21" width="20.5" style="28" customWidth="1"/>
-    <col min="22" max="16384" width="8.796875" style="15"/>
+    <col min="1" max="3" width="19.3984375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="5.09765625" style="18" customWidth="1"/>
+    <col min="6" max="7" width="13.59765625" style="15" customWidth="1"/>
+    <col min="8" max="17" width="13.59765625" style="13" customWidth="1"/>
+    <col min="18" max="18" width="5.09765625" style="18" customWidth="1"/>
+    <col min="19" max="19" width="14.19921875" style="13" customWidth="1"/>
+    <col min="20" max="20" width="16.19921875" style="13" customWidth="1"/>
+    <col min="21" max="21" width="20.5" style="26" customWidth="1"/>
+    <col min="22" max="16384" width="8.796875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="F1" s="23" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="F1" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="S1" s="25" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="S1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="26"/>
-      <c r="U1" s="27"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="25"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="30"/>
+      <c r="F2" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="L2" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="44" t="s">
+      <c r="N2" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="O2" s="44" t="s">
+      <c r="O2" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="44" t="s">
+      <c r="P2" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="Q2" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="30" t="s">
+      <c r="R2" s="33"/>
+      <c r="S2" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="T2" s="30" t="s">
+      <c r="T2" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="U2" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="45" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31" t="s">
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="L3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="M3" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P3" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="Q3" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="35"/>
-      <c r="S3" s="30" t="s">
+      <c r="R3" s="33"/>
+      <c r="S3" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="30" t="s">
+      <c r="T3" s="28" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="28">
         <v>0.1143</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="34">
         <v>1.1867037679233332</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="43">
         <v>7.9947670615597044E-2</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33">
+      <c r="E4" s="30"/>
+      <c r="F4" s="31">
         <v>1</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="31">
         <v>1</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="29">
         <v>19.579999999999998</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="29">
         <v>1020</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="29">
         <v>26.5</v>
       </c>
-      <c r="K4" s="30">
+      <c r="K4" s="28">
         <v>100.14</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="28">
         <v>7.9200400000000002</v>
       </c>
-      <c r="M4" s="28">
+      <c r="M4" s="26">
         <v>0.24751000000000001</v>
       </c>
-      <c r="N4" s="30">
+      <c r="N4" s="28">
         <v>86.35</v>
       </c>
-      <c r="O4" s="30">
+      <c r="O4" s="28">
         <v>6.8293999999999997</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="26">
         <v>0.21343000000000001</v>
       </c>
-      <c r="Q4" s="45">
+      <c r="Q4" s="43">
         <v>2.72</v>
       </c>
-      <c r="R4" s="37"/>
-      <c r="S4" s="30">
-        <f>(M4-P4)/Q4</f>
+      <c r="R4" s="35"/>
+      <c r="S4" s="28">
+        <f t="shared" ref="S4:S15" si="0">(M4-P4)/Q4</f>
         <v>1.2529411764705881E-2</v>
       </c>
-      <c r="T4" s="30">
-        <f>((D4)*(1/14.00672))/Q4</f>
+      <c r="T4" s="28">
+        <f t="shared" ref="T4:T9" si="1">((D4)*(1/14.00672))/Q4</f>
         <v>2.0984588798531388E-3</v>
       </c>
-      <c r="U4" s="28">
+      <c r="U4" s="26">
         <f>S4/T4</f>
         <v>5.9707683028712744</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="28">
         <v>0.1095</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="34">
         <v>1.136866258968156</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="43">
         <v>3.0110161660419799E-2</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="33">
+      <c r="E5" s="30"/>
+      <c r="F5" s="31">
         <v>1</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="31">
         <v>2</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="29">
         <v>19.579999999999998</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="29">
         <v>1020</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="29">
         <v>26.5</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="28">
         <v>98.01</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="28">
         <v>7.7515799999999997</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="26">
         <v>0.24224999999999999</v>
       </c>
-      <c r="N5" s="30">
+      <c r="N5" s="28">
         <v>91.39</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="28">
         <v>7.2280100000000003</v>
       </c>
-      <c r="P5" s="28">
+      <c r="P5" s="26">
         <v>0.22588</v>
       </c>
-      <c r="Q5" s="45">
+      <c r="Q5" s="43">
         <v>2.72</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="30">
-        <f>(M5-P5)/Q5</f>
+      <c r="R5" s="33"/>
+      <c r="S5" s="28">
+        <f t="shared" si="0"/>
         <v>6.0183823529411746E-3</v>
       </c>
-      <c r="T5" s="30">
-        <f>((D5)*(1/14.00672))/Q5</f>
+      <c r="T5" s="28">
+        <f t="shared" si="1"/>
         <v>7.903286690356012E-4</v>
       </c>
-      <c r="U5" s="28">
-        <f t="shared" ref="U5:U15" si="0">S5/T5</f>
+      <c r="U5" s="26">
+        <f t="shared" ref="U5:U15" si="2">S5/T5</f>
         <v>7.6150373746217603</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="28">
         <v>0.1157</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="34">
         <v>1.2012397080352599</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="43">
         <v>9.4483610727523759E-2</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33">
+      <c r="E6" s="30"/>
+      <c r="F6" s="31">
         <v>1</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="31">
         <v>3</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="29">
         <v>19.579999999999998</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="29">
         <v>1020</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="29">
         <v>26.5</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="28">
         <v>98.17</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="28">
         <v>7.76424</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M6" s="26">
         <v>0.24263999999999999</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="28">
         <v>81.27</v>
       </c>
-      <c r="O6" s="30">
+      <c r="O6" s="28">
         <v>6.4276200000000001</v>
       </c>
-      <c r="P6" s="28">
+      <c r="P6" s="26">
         <v>0.20086999999999999</v>
       </c>
-      <c r="Q6" s="45">
+      <c r="Q6" s="43">
         <v>2.72</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="30">
-        <f>(M6-P6)/Q6</f>
+      <c r="R6" s="33"/>
+      <c r="S6" s="28">
+        <f t="shared" si="0"/>
         <v>1.5356617647058823E-2</v>
       </c>
-      <c r="T6" s="30">
-        <f>((D6)*(1/14.00672))/Q6</f>
+      <c r="T6" s="28">
+        <f t="shared" si="1"/>
         <v>2.4799968580082547E-3</v>
       </c>
-      <c r="U6" s="28">
+      <c r="U6" s="26">
+        <f t="shared" si="2"/>
+        <v>6.1921923801920027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="28">
+        <v>0.11360000000000001</v>
+      </c>
+      <c r="C7" s="34">
+        <v>1.17943579786737</v>
+      </c>
+      <c r="D7" s="43">
+        <v>5.3990634701442275E-2</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31">
+        <v>1</v>
+      </c>
+      <c r="G7" s="31">
+        <v>5</v>
+      </c>
+      <c r="H7" s="29">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="I7" s="29">
+        <v>1020</v>
+      </c>
+      <c r="J7" s="29">
+        <v>26.5</v>
+      </c>
+      <c r="K7" s="28">
+        <v>103.65</v>
+      </c>
+      <c r="L7" s="28">
+        <v>8.1976499999999994</v>
+      </c>
+      <c r="M7" s="26">
+        <v>0.25618999999999997</v>
+      </c>
+      <c r="N7" s="28">
+        <v>83.89</v>
+      </c>
+      <c r="O7" s="28">
+        <v>6.63483</v>
+      </c>
+      <c r="P7" s="26">
+        <v>0.20735000000000001</v>
+      </c>
+      <c r="Q7" s="43">
+        <v>2.72</v>
+      </c>
+      <c r="R7" s="33"/>
+      <c r="S7" s="28">
         <f t="shared" si="0"/>
-        <v>6.1921923801920027</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="30">
-        <v>0.11360000000000001</v>
-      </c>
-      <c r="C7" s="36">
-        <v>1.17943579786737</v>
-      </c>
-      <c r="D7" s="45">
-        <v>5.3990634701442275E-2</v>
-      </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33">
+        <v>1.7955882352941162E-2</v>
+      </c>
+      <c r="T7" s="28">
+        <f t="shared" si="1"/>
+        <v>1.4171410617190058E-3</v>
+      </c>
+      <c r="U7" s="26">
+        <f t="shared" si="2"/>
+        <v>12.670497551711968</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="28">
+        <v>0.1086</v>
+      </c>
+      <c r="C8" s="34">
+        <v>1.1275217260390602</v>
+      </c>
+      <c r="D8" s="44">
+        <v>2.07656287313251E-3</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37">
         <v>1</v>
       </c>
-      <c r="G7" s="33">
-        <v>5</v>
-      </c>
-      <c r="H7" s="31">
+      <c r="G8" s="37">
+        <v>6</v>
+      </c>
+      <c r="H8" s="29">
         <v>19.579999999999998</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I8" s="29">
         <v>1020</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J8" s="29">
         <v>26.5</v>
       </c>
-      <c r="K7" s="30">
-        <v>103.65</v>
-      </c>
-      <c r="L7" s="30">
-        <v>8.1976499999999994</v>
-      </c>
-      <c r="M7" s="28">
-        <v>0.25618999999999997</v>
-      </c>
-      <c r="N7" s="30">
-        <v>83.89</v>
-      </c>
-      <c r="O7" s="30">
-        <v>6.63483</v>
-      </c>
-      <c r="P7" s="28">
-        <v>0.20735000000000001</v>
-      </c>
-      <c r="Q7" s="45">
+      <c r="K8" s="28">
+        <v>100.5</v>
+      </c>
+      <c r="L8" s="28">
+        <v>7.9485099999999997</v>
+      </c>
+      <c r="M8" s="26">
+        <v>0.24840000000000001</v>
+      </c>
+      <c r="N8" s="28">
+        <v>95.42</v>
+      </c>
+      <c r="O8" s="28">
+        <v>7.5467399999999998</v>
+      </c>
+      <c r="P8" s="26">
+        <v>0.23583999999999999</v>
+      </c>
+      <c r="Q8" s="43">
         <v>2.72</v>
       </c>
-      <c r="R7" s="35"/>
-      <c r="S7" s="30">
-        <f>(M7-P7)/Q7</f>
-        <v>1.7955882352941162E-2</v>
-      </c>
-      <c r="T7" s="30">
-        <f>((D7)*(1/14.00672))/Q7</f>
-        <v>1.4171410617190058E-3</v>
-      </c>
-      <c r="U7" s="28">
+      <c r="R8" s="33"/>
+      <c r="S8" s="28">
         <f t="shared" si="0"/>
-        <v>12.670497551711968</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="30">
-        <v>0.1086</v>
-      </c>
-      <c r="C8" s="36">
-        <v>1.1275217260390602</v>
-      </c>
-      <c r="D8" s="46">
-        <v>2.07656287313251E-3</v>
-      </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39">
+        <v>4.6176470588235345E-3</v>
+      </c>
+      <c r="T8" s="38">
+        <f t="shared" si="1"/>
+        <v>5.4505425450734011E-5</v>
+      </c>
+      <c r="U8" s="27">
+        <f t="shared" si="2"/>
+        <v>84.719035227003261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0.11219999999999999</v>
+      </c>
+      <c r="C9" s="34">
+        <v>1.164899857755443</v>
+      </c>
+      <c r="D9" s="43">
+        <v>5.1914071828309538E-3</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31">
         <v>1</v>
       </c>
-      <c r="G8" s="39">
-        <v>6</v>
-      </c>
-      <c r="H8" s="31">
+      <c r="G9" s="31">
+        <v>7</v>
+      </c>
+      <c r="H9" s="29">
         <v>19.579999999999998</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I9" s="29">
         <v>1020</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J9" s="29">
         <v>26.5</v>
       </c>
-      <c r="K8" s="30">
-        <v>100.5</v>
-      </c>
-      <c r="L8" s="30">
-        <v>7.9485099999999997</v>
-      </c>
-      <c r="M8" s="28">
-        <v>0.24840000000000001</v>
-      </c>
-      <c r="N8" s="30">
-        <v>95.42</v>
-      </c>
-      <c r="O8" s="30">
-        <v>7.5467399999999998</v>
-      </c>
-      <c r="P8" s="28">
-        <v>0.23583999999999999</v>
-      </c>
-      <c r="Q8" s="45">
+      <c r="K9" s="28">
+        <v>101.1</v>
+      </c>
+      <c r="L9" s="28">
+        <v>7.9959699999999998</v>
+      </c>
+      <c r="M9" s="26">
+        <v>0.24987999999999999</v>
+      </c>
+      <c r="N9" s="28">
+        <v>94.62</v>
+      </c>
+      <c r="O9" s="28">
+        <v>7.4834699999999996</v>
+      </c>
+      <c r="P9" s="26">
+        <v>0.23386999999999999</v>
+      </c>
+      <c r="Q9" s="43">
         <v>2.72</v>
       </c>
-      <c r="R8" s="35"/>
-      <c r="S8" s="30">
-        <f>(M8-P8)/Q8</f>
-        <v>4.6176470588235345E-3</v>
-      </c>
-      <c r="T8" s="40">
-        <f>((D8)*(1/14.00672))/Q8</f>
-        <v>5.4505425450734011E-5</v>
-      </c>
-      <c r="U8" s="29">
+      <c r="R9" s="33"/>
+      <c r="S9" s="28">
         <f t="shared" si="0"/>
-        <v>84.719035227003261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="30">
-        <v>0.11219999999999999</v>
-      </c>
-      <c r="C9" s="36">
-        <v>1.164899857755443</v>
-      </c>
-      <c r="D9" s="45">
-        <v>5.1914071828309538E-3</v>
-      </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33">
+        <v>5.886029411764704E-3</v>
+      </c>
+      <c r="T9" s="28">
+        <f t="shared" si="1"/>
+        <v>1.362635636268266E-4</v>
+      </c>
+      <c r="U9" s="26">
+        <f t="shared" si="2"/>
+        <v>43.195915731987391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0.1166</v>
+      </c>
+      <c r="C10" s="34">
+        <v>1.2105842409643557</v>
+      </c>
+      <c r="D10" s="43">
+        <v>5.0875790391743614E-2</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31">
+        <v>2</v>
+      </c>
+      <c r="G10" s="31">
         <v>1</v>
       </c>
-      <c r="G9" s="33">
-        <v>7</v>
-      </c>
-      <c r="H9" s="31">
-        <v>19.579999999999998</v>
-      </c>
-      <c r="I9" s="31">
-        <v>1020</v>
-      </c>
-      <c r="J9" s="31">
-        <v>26.5</v>
-      </c>
-      <c r="K9" s="30">
-        <v>101.1</v>
-      </c>
-      <c r="L9" s="30">
-        <v>7.9959699999999998</v>
-      </c>
-      <c r="M9" s="28">
-        <v>0.24987999999999999</v>
-      </c>
-      <c r="N9" s="30">
-        <v>94.62</v>
-      </c>
-      <c r="O9" s="30">
-        <v>7.4834699999999996</v>
-      </c>
-      <c r="P9" s="28">
-        <v>0.23386999999999999</v>
-      </c>
-      <c r="Q9" s="45">
-        <v>2.72</v>
-      </c>
-      <c r="R9" s="35"/>
-      <c r="S9" s="30">
-        <f>(M9-P9)/Q9</f>
-        <v>5.886029411764704E-3</v>
-      </c>
-      <c r="T9" s="30">
-        <f>((D9)*(1/14.00672))/Q9</f>
-        <v>1.362635636268266E-4</v>
-      </c>
-      <c r="U9" s="28">
+      <c r="H10" s="29">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="I10" s="29">
+        <v>999</v>
+      </c>
+      <c r="J10" s="29">
+        <v>26.9</v>
+      </c>
+      <c r="K10" s="28">
+        <v>100.87</v>
+      </c>
+      <c r="L10" s="28">
+        <v>7.9777800000000001</v>
+      </c>
+      <c r="M10" s="26">
+        <v>0.24931</v>
+      </c>
+      <c r="N10" s="28">
+        <v>93.57</v>
+      </c>
+      <c r="O10" s="28">
+        <v>7.4004200000000004</v>
+      </c>
+      <c r="P10" s="26">
+        <v>0.23127</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>2.23</v>
+      </c>
+      <c r="R10" s="33"/>
+      <c r="S10" s="28">
         <f t="shared" si="0"/>
-        <v>43.195915731987391</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="30">
-        <v>0.1166</v>
-      </c>
-      <c r="C10" s="36">
-        <v>1.2105842409643557</v>
-      </c>
-      <c r="D10" s="45">
-        <v>5.0875790391743614E-2</v>
-      </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33">
+        <v>8.0896860986547081E-3</v>
+      </c>
+      <c r="T10" s="28">
+        <f t="shared" ref="T10:T15" si="3">((D10)*(1/14.00672))/Q10</f>
+        <v>1.6288078708684792E-3</v>
+      </c>
+      <c r="U10" s="26">
+        <f t="shared" si="2"/>
+        <v>4.9666300386559978</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="28">
+        <v>0.11890000000000001</v>
+      </c>
+      <c r="C11" s="34">
+        <v>1.2344647140053784</v>
+      </c>
+      <c r="D11" s="43">
+        <v>7.4756263432766312E-2</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31">
         <v>2</v>
       </c>
-      <c r="G10" s="33">
-        <v>1</v>
-      </c>
-      <c r="H10" s="31">
+      <c r="G11" s="31">
+        <v>2</v>
+      </c>
+      <c r="H11" s="29">
         <v>19.600000000000001</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I11" s="29">
         <v>999</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J11" s="29">
         <v>26.9</v>
       </c>
-      <c r="K10" s="30">
-        <v>100.87</v>
-      </c>
-      <c r="L10" s="30">
-        <v>7.9777800000000001</v>
-      </c>
-      <c r="M10" s="28">
-        <v>0.24931</v>
-      </c>
-      <c r="N10" s="30">
-        <v>93.57</v>
-      </c>
-      <c r="O10" s="30">
-        <v>7.4004200000000004</v>
-      </c>
-      <c r="P10" s="28">
-        <v>0.23127</v>
-      </c>
-      <c r="Q10" s="28">
+      <c r="K11" s="28">
+        <v>99.81</v>
+      </c>
+      <c r="L11" s="28">
+        <v>7.8939399999999997</v>
+      </c>
+      <c r="M11" s="26">
+        <v>0.24668999999999999</v>
+      </c>
+      <c r="N11" s="28">
+        <v>88.14</v>
+      </c>
+      <c r="O11" s="28">
+        <v>6.9709700000000003</v>
+      </c>
+      <c r="P11" s="26">
+        <v>0.21784999999999999</v>
+      </c>
+      <c r="Q11" s="26">
         <v>2.23</v>
       </c>
-      <c r="R10" s="35"/>
-      <c r="S10" s="30">
-        <f>(M10-P10)/Q10</f>
-        <v>8.0896860986547081E-3</v>
-      </c>
-      <c r="T10" s="30">
-        <f t="shared" ref="T10:T15" si="1">((D10)*(1/14.00672))/Q10</f>
-        <v>1.6288078708684792E-3</v>
-      </c>
-      <c r="U10" s="28">
+      <c r="R11" s="33"/>
+      <c r="S11" s="28">
         <f t="shared" si="0"/>
-        <v>4.9666300386559978</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="30">
-        <v>0.11890000000000001</v>
-      </c>
-      <c r="C11" s="36">
-        <v>1.2344647140053784</v>
-      </c>
-      <c r="D11" s="45">
-        <v>7.4756263432766312E-2</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33">
+        <v>1.293273542600897E-2</v>
+      </c>
+      <c r="T11" s="28">
+        <f t="shared" si="3"/>
+        <v>2.3933503408679756E-3</v>
+      </c>
+      <c r="U11" s="26">
+        <f t="shared" si="2"/>
+        <v>5.4036115002364289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="28">
+        <v>0.112</v>
+      </c>
+      <c r="C12" s="34">
+        <v>1.1628232948823107</v>
+      </c>
+      <c r="D12" s="43">
+        <v>3.1148443096986611E-3</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31">
         <v>2</v>
       </c>
-      <c r="G11" s="33">
-        <v>2</v>
-      </c>
-      <c r="H11" s="31">
+      <c r="G12" s="31">
+        <v>3</v>
+      </c>
+      <c r="H12" s="29">
         <v>19.600000000000001</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I12" s="29">
         <v>999</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J12" s="29">
         <v>26.9</v>
       </c>
-      <c r="K11" s="30">
-        <v>99.81</v>
-      </c>
-      <c r="L11" s="30">
-        <v>7.8939399999999997</v>
-      </c>
-      <c r="M11" s="28">
-        <v>0.24668999999999999</v>
-      </c>
-      <c r="N11" s="30">
-        <v>88.14</v>
-      </c>
-      <c r="O11" s="30">
-        <v>6.9709700000000003</v>
-      </c>
-      <c r="P11" s="28">
-        <v>0.21784999999999999</v>
-      </c>
-      <c r="Q11" s="28">
+      <c r="K12" s="28">
+        <v>98.64</v>
+      </c>
+      <c r="L12" s="28">
+        <v>7.8014099999999997</v>
+      </c>
+      <c r="M12" s="26">
+        <v>0.24379999999999999</v>
+      </c>
+      <c r="N12" s="28">
+        <v>86.76</v>
+      </c>
+      <c r="O12" s="28">
+        <v>6.8618199999999998</v>
+      </c>
+      <c r="P12" s="26">
+        <v>0.21443999999999999</v>
+      </c>
+      <c r="Q12" s="26">
         <v>2.23</v>
       </c>
-      <c r="R11" s="35"/>
-      <c r="S11" s="30">
-        <f>(M11-P11)/Q11</f>
-        <v>1.293273542600897E-2</v>
-      </c>
-      <c r="T11" s="30">
-        <f t="shared" si="1"/>
-        <v>2.3933503408679756E-3</v>
-      </c>
-      <c r="U11" s="28">
+      <c r="R12" s="33"/>
+      <c r="S12" s="28">
         <f t="shared" si="0"/>
-        <v>5.4036115002364289</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="30">
-        <v>0.112</v>
-      </c>
-      <c r="C12" s="36">
-        <v>1.1628232948823107</v>
-      </c>
-      <c r="D12" s="45">
-        <v>3.1148443096986611E-3</v>
-      </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33">
-        <v>2</v>
-      </c>
-      <c r="G12" s="33">
-        <v>3</v>
-      </c>
-      <c r="H12" s="31">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I12" s="31">
-        <v>999</v>
-      </c>
-      <c r="J12" s="31">
-        <v>26.9</v>
-      </c>
-      <c r="K12" s="30">
-        <v>98.64</v>
-      </c>
-      <c r="L12" s="30">
-        <v>7.8014099999999997</v>
-      </c>
-      <c r="M12" s="28">
-        <v>0.24379999999999999</v>
-      </c>
-      <c r="N12" s="30">
-        <v>86.76</v>
-      </c>
-      <c r="O12" s="30">
-        <v>6.8618199999999998</v>
-      </c>
-      <c r="P12" s="28">
-        <v>0.21443999999999999</v>
-      </c>
-      <c r="Q12" s="28">
-        <v>2.23</v>
-      </c>
-      <c r="R12" s="35"/>
-      <c r="S12" s="30">
-        <f>(M12-P12)/Q12</f>
         <v>1.3165919282511209E-2</v>
       </c>
-      <c r="T12" s="30">
-        <f t="shared" si="1"/>
+      <c r="T12" s="28">
+        <f t="shared" si="3"/>
         <v>9.9722930869501061E-5</v>
       </c>
-      <c r="U12" s="28">
+      <c r="U12" s="26">
         <f>S12/T12</f>
         <v>132.02499332616216</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="28">
         <v>0.11550000000000001</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="34">
         <v>1.1991631451621276</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D13" s="43">
         <v>3.945469458951556E-2</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33">
+      <c r="E13" s="30"/>
+      <c r="F13" s="31">
         <v>2</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="31">
         <v>5</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="29">
         <v>19.600000000000001</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="29">
         <v>999</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="29">
         <v>26.9</v>
       </c>
-      <c r="K13" s="30">
+      <c r="K13" s="28">
         <v>99.34</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="28">
         <v>7.85677</v>
       </c>
-      <c r="M13" s="28">
+      <c r="M13" s="26">
         <v>0.24553</v>
       </c>
-      <c r="N13" s="30">
+      <c r="N13" s="28">
         <v>88.9</v>
       </c>
-      <c r="O13" s="30">
+      <c r="O13" s="28">
         <v>7.0310699999999997</v>
       </c>
-      <c r="P13" s="28">
+      <c r="P13" s="26">
         <v>0.21973000000000001</v>
       </c>
-      <c r="Q13" s="28">
+      <c r="Q13" s="26">
         <v>2.23</v>
       </c>
-      <c r="R13" s="35"/>
-      <c r="S13" s="30">
-        <f>(M13-P13)/Q13</f>
+      <c r="R13" s="33"/>
+      <c r="S13" s="28">
+        <f t="shared" si="0"/>
         <v>1.1569506726457394E-2</v>
       </c>
-      <c r="T13" s="30">
-        <f t="shared" si="1"/>
+      <c r="T13" s="28">
+        <f t="shared" si="3"/>
         <v>1.2631571243469873E-3</v>
       </c>
-      <c r="U13" s="28">
+      <c r="U13" s="26">
+        <f t="shared" si="2"/>
+        <v>9.1591984112336515</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="28">
+        <v>0.1132</v>
+      </c>
+      <c r="C14" s="34">
+        <v>1.1752826721211052</v>
+      </c>
+      <c r="D14" s="43">
+        <v>1.5574221548493083E-2</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="37">
+        <v>2</v>
+      </c>
+      <c r="G14" s="37">
+        <v>6</v>
+      </c>
+      <c r="H14" s="29">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="I14" s="29">
+        <v>999</v>
+      </c>
+      <c r="J14" s="29">
+        <v>26.9</v>
+      </c>
+      <c r="K14" s="28">
+        <v>99.43</v>
+      </c>
+      <c r="L14" s="28">
+        <v>7.8638899999999996</v>
+      </c>
+      <c r="M14" s="26">
+        <v>0.24576000000000001</v>
+      </c>
+      <c r="N14" s="28">
+        <v>86.68</v>
+      </c>
+      <c r="O14" s="28">
+        <v>6.8554899999999996</v>
+      </c>
+      <c r="P14" s="26">
+        <v>0.21424000000000001</v>
+      </c>
+      <c r="Q14" s="26">
+        <v>2.23</v>
+      </c>
+      <c r="R14" s="33"/>
+      <c r="S14" s="28">
         <f t="shared" si="0"/>
-        <v>9.1591984112336515</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+        <v>1.4134529147982059E-2</v>
+      </c>
+      <c r="T14" s="28">
+        <f t="shared" si="3"/>
+        <v>4.9861465434749826E-4</v>
+      </c>
+      <c r="U14" s="26">
+        <f t="shared" si="2"/>
+        <v>28.347600746871183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="39">
+        <v>0.11550000000000001</v>
+      </c>
+      <c r="C15" s="34">
+        <v>1.1991631451621276</v>
+      </c>
+      <c r="D15" s="43">
+        <v>3.0110161660419577E-2</v>
+      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31">
+        <v>2</v>
+      </c>
+      <c r="G15" s="31">
+        <v>7</v>
+      </c>
+      <c r="H15" s="29">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="I15" s="29">
+        <v>999</v>
+      </c>
+      <c r="J15" s="29">
+        <v>26.9</v>
+      </c>
+      <c r="K15" s="28">
+        <v>99.43</v>
+      </c>
+      <c r="L15" s="28">
+        <v>7.8638899999999996</v>
+      </c>
+      <c r="M15" s="26">
+        <v>0.24576000000000001</v>
+      </c>
+      <c r="N15" s="28">
+        <v>82.24</v>
+      </c>
+      <c r="O15" s="28">
+        <v>6.50434</v>
+      </c>
+      <c r="P15" s="26">
+        <v>0.20327000000000001</v>
+      </c>
+      <c r="Q15" s="26">
+        <v>2.23</v>
+      </c>
+      <c r="R15" s="33"/>
+      <c r="S15" s="28">
+        <f t="shared" si="0"/>
+        <v>1.9053811659192826E-2</v>
+      </c>
+      <c r="T15" s="28">
+        <f t="shared" si="3"/>
+        <v>9.6398833173848427E-4</v>
+      </c>
+      <c r="U15" s="26">
+        <f t="shared" si="2"/>
+        <v>19.76560403467813</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="39">
+        <v>0.11840000000000001</v>
+      </c>
+      <c r="C16" s="34">
+        <v>1.2292733068225474</v>
+      </c>
+      <c r="D16" s="29">
+        <v>6.0220323320839375E-2</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="39">
+        <v>0.1172</v>
+      </c>
+      <c r="C17" s="34">
+        <v>1.216813929583753</v>
+      </c>
+      <c r="D17" s="29">
+        <v>5.9182041884273229E-2</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="30">
-        <v>0.1132</v>
-      </c>
-      <c r="C14" s="36">
-        <v>1.1752826721211052</v>
-      </c>
-      <c r="D14" s="45">
-        <v>1.5574221548493083E-2</v>
-      </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="39">
-        <v>2</v>
-      </c>
-      <c r="G14" s="39">
-        <v>6</v>
-      </c>
-      <c r="H14" s="31">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I14" s="31">
-        <v>999</v>
-      </c>
-      <c r="J14" s="31">
-        <v>26.9</v>
-      </c>
-      <c r="K14" s="30">
-        <v>99.43</v>
-      </c>
-      <c r="L14" s="30">
-        <v>7.8638899999999996</v>
-      </c>
-      <c r="M14" s="28">
-        <v>0.24576000000000001</v>
-      </c>
-      <c r="N14" s="30">
-        <v>86.68</v>
-      </c>
-      <c r="O14" s="30">
-        <v>6.8554899999999996</v>
-      </c>
-      <c r="P14" s="28">
-        <v>0.21424000000000001</v>
-      </c>
-      <c r="Q14" s="28">
-        <v>2.23</v>
-      </c>
-      <c r="R14" s="35"/>
-      <c r="S14" s="30">
-        <f>(M14-P14)/Q14</f>
-        <v>1.4134529147982059E-2</v>
-      </c>
-      <c r="T14" s="30">
-        <f t="shared" si="1"/>
-        <v>4.9861465434749826E-4</v>
-      </c>
-      <c r="U14" s="28">
-        <f t="shared" si="0"/>
-        <v>28.347600746871183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="41">
-        <v>0.11550000000000001</v>
-      </c>
-      <c r="C15" s="36">
-        <v>1.1991631451621276</v>
-      </c>
-      <c r="D15" s="45">
-        <v>3.0110161660419577E-2</v>
-      </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33">
-        <v>2</v>
-      </c>
-      <c r="G15" s="33">
-        <v>7</v>
-      </c>
-      <c r="H15" s="31">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I15" s="31">
-        <v>999</v>
-      </c>
-      <c r="J15" s="31">
-        <v>26.9</v>
-      </c>
-      <c r="K15" s="30">
-        <v>99.43</v>
-      </c>
-      <c r="L15" s="30">
-        <v>7.8638899999999996</v>
-      </c>
-      <c r="M15" s="28">
-        <v>0.24576000000000001</v>
-      </c>
-      <c r="N15" s="30">
-        <v>82.24</v>
-      </c>
-      <c r="O15" s="30">
-        <v>6.50434</v>
-      </c>
-      <c r="P15" s="28">
-        <v>0.20327000000000001</v>
-      </c>
-      <c r="Q15" s="28">
-        <v>2.23</v>
-      </c>
-      <c r="R15" s="35"/>
-      <c r="S15" s="30">
-        <f>(M15-P15)/Q15</f>
-        <v>1.9053811659192826E-2</v>
-      </c>
-      <c r="T15" s="30">
-        <f t="shared" si="1"/>
-        <v>9.6398833173848427E-4</v>
-      </c>
-      <c r="U15" s="28">
-        <f t="shared" si="0"/>
-        <v>19.76560403467813</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="41">
-        <v>0.11840000000000001</v>
-      </c>
-      <c r="C16" s="36">
-        <v>1.2292733068225474</v>
-      </c>
-      <c r="D16" s="31">
-        <v>6.0220323320839375E-2</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+      <c r="B18" s="39">
+        <v>0.1162</v>
+      </c>
+      <c r="C18" s="34">
+        <v>1.2064311152180911</v>
+      </c>
+      <c r="D18" s="29">
+        <v>4.8799227518611321E-2</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="39">
+        <v>0.1145</v>
+      </c>
+      <c r="C19" s="34">
+        <v>1.1887803307964657</v>
+      </c>
+      <c r="D19" s="29">
+        <v>3.1148443096985945E-2</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="41">
-        <v>0.1172</v>
-      </c>
-      <c r="C17" s="36">
-        <v>1.216813929583753</v>
-      </c>
-      <c r="D17" s="31">
-        <v>5.9182041884273229E-2</v>
-      </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="41">
-        <v>0.1162</v>
-      </c>
-      <c r="C18" s="36">
-        <v>1.2064311152180911</v>
-      </c>
-      <c r="D18" s="31">
-        <v>4.8799227518611321E-2</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="41">
-        <v>0.1145</v>
-      </c>
-      <c r="C19" s="36">
-        <v>1.1887803307964657</v>
-      </c>
-      <c r="D19" s="31">
-        <v>3.1148443096985945E-2</v>
-      </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="41">
+      <c r="B20" s="39">
         <v>0.1164</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="34">
         <v>1.2085076780912234</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="29">
         <v>5.0875790391743614E-2</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K21" s="15" t="s">
+      <c r="E20" s="19"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="K21" s="13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K22" s="15" t="s">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="K22" s="13" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K24" s="15" t="s">
+      <c r="U22" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="V22" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="U23" s="26">
+        <f>AVERAGE(U4:U7,U9:U11,U13:U15)</f>
+        <v>14.328705607305977</v>
+      </c>
+      <c r="V23" s="13">
+        <f>_xlfn.STDEV.S(U4:U7,U9:U11,U13:U15)</f>
+        <v>12.637315259991174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="K24" s="13" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor adjust of excretion date
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Excretion/20211026_Excretion_raw.xlsx
+++ b/RAnalysis/Data/Excretion/20211026_Excretion_raw.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2352" yWindow="0" windowWidth="21864" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="3528" yWindow="0" windowWidth="21864" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Excretion 10-26-21" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="F8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
   <si>
     <t>Standard Addition Determination of Ammonia-N Concentration in Seawater Blank</t>
   </si>
@@ -315,6 +315,12 @@
   <si>
     <t>sd</t>
   </si>
+  <si>
+    <t>whole DW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">length </t>
+  </si>
 </sst>
 </file>
 
@@ -325,7 +331,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,8 +431,26 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,6 +499,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CB9C"/>
+        <bgColor rgb="FFF9CB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -488,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -503,26 +533,11 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -555,13 +570,9 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -571,13 +582,55 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,6 +706,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -931,6 +985,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1034,6 +1089,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -1096,6 +1152,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -1392,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:M3"/>
+    <sheetView topLeftCell="C7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K31" activeCellId="3" sqref="K13:L18 K21:L23 K25:L29 K31:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1409,15 +1466,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6984,1056 +7041,1195 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="19.3984375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.796875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="5.09765625" style="18" customWidth="1"/>
-    <col min="6" max="7" width="13.59765625" style="15" customWidth="1"/>
-    <col min="8" max="17" width="13.59765625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="5.09765625" style="18" customWidth="1"/>
-    <col min="19" max="19" width="14.19921875" style="13" customWidth="1"/>
-    <col min="20" max="20" width="16.19921875" style="13" customWidth="1"/>
-    <col min="21" max="21" width="20.5" style="26" customWidth="1"/>
-    <col min="22" max="16384" width="8.796875" style="13"/>
+    <col min="1" max="5" width="19.3984375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="17.796875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="5.09765625" style="20" customWidth="1"/>
+    <col min="8" max="9" width="13.59765625" style="18" customWidth="1"/>
+    <col min="10" max="19" width="13.59765625" style="15" customWidth="1"/>
+    <col min="20" max="20" width="5.09765625" style="20" customWidth="1"/>
+    <col min="21" max="21" width="14.19921875" style="15" customWidth="1"/>
+    <col min="22" max="22" width="16.19921875" style="15" customWidth="1"/>
+    <col min="23" max="23" width="20.5" style="14" customWidth="1"/>
+    <col min="24" max="16384" width="8.796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="F1" s="21" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="S1" s="23" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="U1" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="24"/>
-      <c r="U1" s="25"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="V1" s="38"/>
+      <c r="W1" s="13"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="D2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="E2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="F2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="I2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="J2" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="K2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="L2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="M2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="N2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="O2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="42" t="s">
+      <c r="P2" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="O2" s="42" t="s">
+      <c r="Q2" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="42" t="s">
+      <c r="R2" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="S2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="28" t="s">
+      <c r="U2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="V2" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="W2" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="43" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29" t="s">
+      <c r="G3" s="17"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="L3" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="M3" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="N3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="O3" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="P3" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="28" t="s">
+      <c r="Q3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="R3" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="Q3" s="26" t="s">
+      <c r="S3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="33"/>
-      <c r="S3" s="28" t="s">
+      <c r="U3" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="28" t="s">
+      <c r="V3" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="40">
+        <v>12.61</v>
+      </c>
+      <c r="C4" s="41">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="D4" s="15">
         <v>0.1143</v>
       </c>
-      <c r="C4" s="34">
+      <c r="E4" s="21">
         <v>1.1867037679233332</v>
       </c>
-      <c r="D4" s="43">
+      <c r="F4" s="42">
         <v>7.9947670615597044E-2</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31">
+      <c r="G4" s="17"/>
+      <c r="H4" s="18">
         <v>1</v>
       </c>
-      <c r="G4" s="31">
+      <c r="I4" s="18">
         <v>1</v>
       </c>
-      <c r="H4" s="29">
+      <c r="J4" s="16">
         <v>19.579999999999998</v>
       </c>
-      <c r="I4" s="29">
+      <c r="K4" s="16">
         <v>1020</v>
       </c>
-      <c r="J4" s="29">
+      <c r="L4" s="16">
         <v>26.5</v>
       </c>
-      <c r="K4" s="28">
+      <c r="M4" s="15">
         <v>100.14</v>
       </c>
-      <c r="L4" s="28">
+      <c r="N4" s="15">
         <v>7.9200400000000002</v>
       </c>
-      <c r="M4" s="26">
+      <c r="O4" s="14">
         <v>0.24751000000000001</v>
       </c>
-      <c r="N4" s="28">
+      <c r="P4" s="15">
         <v>86.35</v>
       </c>
-      <c r="O4" s="28">
+      <c r="Q4" s="15">
         <v>6.8293999999999997</v>
       </c>
-      <c r="P4" s="26">
+      <c r="R4" s="14">
         <v>0.21343000000000001</v>
       </c>
-      <c r="Q4" s="43">
+      <c r="S4" s="28">
         <v>2.72</v>
       </c>
-      <c r="R4" s="35"/>
-      <c r="S4" s="28">
-        <f t="shared" ref="S4:S15" si="0">(M4-P4)/Q4</f>
+      <c r="T4" s="22"/>
+      <c r="U4" s="15">
+        <f>(O4-R4)/S4</f>
         <v>1.2529411764705881E-2</v>
       </c>
-      <c r="T4" s="28">
-        <f t="shared" ref="T4:T9" si="1">((D4)*(1/14.00672))/Q4</f>
+      <c r="V4" s="15">
+        <f>((F4)*(1/14.00672))/S4</f>
         <v>2.0984588798531388E-3</v>
       </c>
-      <c r="U4" s="26">
-        <f>S4/T4</f>
+      <c r="W4" s="14">
+        <f>U4/V4</f>
         <v>5.9707683028712744</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="40">
+        <v>8.94</v>
+      </c>
+      <c r="C5" s="41">
+        <v>6.9000000000000172E-3</v>
+      </c>
+      <c r="D5" s="15">
         <v>0.1095</v>
       </c>
-      <c r="C5" s="34">
+      <c r="E5" s="21">
         <v>1.136866258968156</v>
       </c>
-      <c r="D5" s="43">
+      <c r="F5" s="42">
         <v>3.0110161660419799E-2</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31">
+      <c r="G5" s="17"/>
+      <c r="H5" s="18">
         <v>1</v>
       </c>
-      <c r="G5" s="31">
+      <c r="I5" s="18">
         <v>2</v>
       </c>
-      <c r="H5" s="29">
+      <c r="J5" s="16">
         <v>19.579999999999998</v>
       </c>
-      <c r="I5" s="29">
+      <c r="K5" s="16">
         <v>1020</v>
       </c>
-      <c r="J5" s="29">
+      <c r="L5" s="16">
         <v>26.5</v>
       </c>
-      <c r="K5" s="28">
+      <c r="M5" s="15">
         <v>98.01</v>
       </c>
-      <c r="L5" s="28">
+      <c r="N5" s="15">
         <v>7.7515799999999997</v>
       </c>
-      <c r="M5" s="26">
+      <c r="O5" s="14">
         <v>0.24224999999999999</v>
       </c>
-      <c r="N5" s="28">
+      <c r="P5" s="15">
         <v>91.39</v>
       </c>
-      <c r="O5" s="28">
+      <c r="Q5" s="15">
         <v>7.2280100000000003</v>
       </c>
-      <c r="P5" s="26">
+      <c r="R5" s="14">
         <v>0.22588</v>
       </c>
-      <c r="Q5" s="43">
+      <c r="S5" s="28">
         <v>2.72</v>
       </c>
-      <c r="R5" s="33"/>
-      <c r="S5" s="28">
+      <c r="U5" s="15">
+        <f>(O5-R5)/S5</f>
+        <v>6.0183823529411746E-3</v>
+      </c>
+      <c r="V5" s="15">
+        <f t="shared" ref="V5:V15" si="0">((F5)*(1/14.00672))/S5</f>
+        <v>7.903286690356012E-4</v>
+      </c>
+      <c r="W5" s="14">
+        <f t="shared" ref="W5:W15" si="1">U5/V5</f>
+        <v>7.6150373746217603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="40">
+        <v>14.07</v>
+      </c>
+      <c r="C6" s="41">
+        <v>1.9399999999999973E-2</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0.1157</v>
+      </c>
+      <c r="E6" s="21">
+        <v>1.2012397080352599</v>
+      </c>
+      <c r="F6" s="42">
+        <v>9.4483610727523759E-2</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18">
+        <v>1</v>
+      </c>
+      <c r="I6" s="18">
+        <v>3</v>
+      </c>
+      <c r="J6" s="16">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="K6" s="16">
+        <v>1020</v>
+      </c>
+      <c r="L6" s="16">
+        <v>26.5</v>
+      </c>
+      <c r="M6" s="15">
+        <v>98.17</v>
+      </c>
+      <c r="N6" s="15">
+        <v>7.76424</v>
+      </c>
+      <c r="O6" s="14">
+        <v>0.24263999999999999</v>
+      </c>
+      <c r="P6" s="15">
+        <v>81.27</v>
+      </c>
+      <c r="Q6" s="15">
+        <v>6.4276200000000001</v>
+      </c>
+      <c r="R6" s="14">
+        <v>0.20086999999999999</v>
+      </c>
+      <c r="S6" s="28">
+        <v>2.72</v>
+      </c>
+      <c r="U6" s="15">
+        <f>(O6-R6)/S6</f>
+        <v>1.5356617647058823E-2</v>
+      </c>
+      <c r="V6" s="15">
         <f t="shared" si="0"/>
-        <v>6.0183823529411746E-3</v>
-      </c>
-      <c r="T5" s="28">
+        <v>2.4799968580082547E-3</v>
+      </c>
+      <c r="W6" s="14">
         <f t="shared" si="1"/>
-        <v>7.903286690356012E-4</v>
-      </c>
-      <c r="U5" s="26">
-        <f t="shared" ref="U5:U15" si="2">S5/T5</f>
-        <v>7.6150373746217603</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+        <v>6.1921923801920027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="40">
+        <v>8.9</v>
+      </c>
+      <c r="C7" s="15">
+        <v>4.300000000000026E-3</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0.11360000000000001</v>
+      </c>
+      <c r="E7" s="21">
+        <v>1.17943579786737</v>
+      </c>
+      <c r="F7" s="42">
+        <v>5.3990634701442275E-2</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18">
+        <v>1</v>
+      </c>
+      <c r="I7" s="18">
+        <v>5</v>
+      </c>
+      <c r="J7" s="16">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="K7" s="16">
+        <v>1020</v>
+      </c>
+      <c r="L7" s="16">
+        <v>26.5</v>
+      </c>
+      <c r="M7" s="15">
+        <v>103.65</v>
+      </c>
+      <c r="N7" s="15">
+        <v>8.1976499999999994</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0.25618999999999997</v>
+      </c>
+      <c r="P7" s="15">
+        <v>83.89</v>
+      </c>
+      <c r="Q7" s="15">
+        <v>6.63483</v>
+      </c>
+      <c r="R7" s="14">
+        <v>0.20735000000000001</v>
+      </c>
+      <c r="S7" s="28">
+        <v>2.72</v>
+      </c>
+      <c r="U7" s="15">
+        <f>(O7-R7)/S7</f>
+        <v>1.7955882352941162E-2</v>
+      </c>
+      <c r="V7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.4171410617190058E-3</v>
+      </c>
+      <c r="W7" s="14">
+        <f t="shared" si="1"/>
+        <v>12.670497551711968</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="40">
+        <v>7.03</v>
+      </c>
+      <c r="C8" s="15">
+        <v>3.0000000000000027E-3</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.1086</v>
+      </c>
+      <c r="E8" s="21">
+        <v>1.1275217260390602</v>
+      </c>
+      <c r="F8" s="43">
+        <v>2.0765628731325148E-3</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24">
+        <v>1</v>
+      </c>
+      <c r="I8" s="24">
+        <v>6</v>
+      </c>
+      <c r="J8" s="16">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="K8" s="16">
+        <v>1020</v>
+      </c>
+      <c r="L8" s="16">
+        <v>26.5</v>
+      </c>
+      <c r="M8" s="15">
+        <v>100.5</v>
+      </c>
+      <c r="N8" s="15">
+        <v>7.9485099999999997</v>
+      </c>
+      <c r="O8" s="14">
+        <v>0.24840000000000001</v>
+      </c>
+      <c r="P8" s="15">
+        <v>95.42</v>
+      </c>
+      <c r="Q8" s="15">
+        <v>7.5467399999999998</v>
+      </c>
+      <c r="R8" s="14">
+        <v>0.23583999999999999</v>
+      </c>
+      <c r="S8" s="28">
+        <v>2.72</v>
+      </c>
+      <c r="U8" s="15">
+        <f>(O8-R8)/S8</f>
+        <v>4.6176470588235345E-3</v>
+      </c>
+      <c r="V8" s="45">
+        <f t="shared" si="0"/>
+        <v>5.4505425450734139E-5</v>
+      </c>
+      <c r="W8" s="44">
+        <f t="shared" si="1"/>
+        <v>84.719035227003062</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="40">
+        <v>7.4</v>
+      </c>
+      <c r="C9" s="40">
+        <v>3.0000000000000027E-3</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="E9" s="21">
+        <v>1.1088326601808687</v>
+      </c>
+      <c r="F9" s="43">
+        <v>-1.6612502985059008E-2</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18">
+        <v>1</v>
+      </c>
+      <c r="I9" s="18">
+        <v>7</v>
+      </c>
+      <c r="J9" s="16">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="K9" s="16">
+        <v>1020</v>
+      </c>
+      <c r="L9" s="16">
+        <v>26.5</v>
+      </c>
+      <c r="M9" s="15">
+        <v>101.1</v>
+      </c>
+      <c r="N9" s="15">
+        <v>7.9959699999999998</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0.24987999999999999</v>
+      </c>
+      <c r="P9" s="15">
+        <v>94.62</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>7.4834699999999996</v>
+      </c>
+      <c r="R9" s="14">
+        <v>0.23386999999999999</v>
+      </c>
+      <c r="S9" s="28">
+        <v>2.72</v>
+      </c>
+      <c r="U9" s="15">
+        <f>(O9-R9)/S9</f>
+        <v>5.886029411764704E-3</v>
+      </c>
+      <c r="V9" s="45">
+        <f t="shared" si="0"/>
+        <v>-4.3604340360584395E-4</v>
+      </c>
+      <c r="W9" s="44">
+        <f t="shared" si="1"/>
+        <v>-13.498723666246097</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="15">
+        <v>8.65</v>
+      </c>
+      <c r="C10" s="40">
+        <v>3.8000000000000256E-3</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0.11219999999999999</v>
+      </c>
+      <c r="E10" s="21">
+        <v>1.164899857755443</v>
+      </c>
+      <c r="F10" s="42">
+        <v>5.1914071828309538E-3</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18">
+        <v>2</v>
+      </c>
+      <c r="I10" s="18">
+        <v>1</v>
+      </c>
+      <c r="J10" s="16">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K10" s="16">
+        <v>999</v>
+      </c>
+      <c r="L10" s="16">
+        <v>26.9</v>
+      </c>
+      <c r="M10" s="15">
+        <v>100.87</v>
+      </c>
+      <c r="N10" s="15">
+        <v>7.9777800000000001</v>
+      </c>
+      <c r="O10" s="14">
+        <v>0.24931</v>
+      </c>
+      <c r="P10" s="15">
+        <v>93.57</v>
+      </c>
+      <c r="Q10" s="15">
+        <v>7.4004200000000004</v>
+      </c>
+      <c r="R10" s="14">
+        <v>0.23127</v>
+      </c>
+      <c r="S10" s="14">
+        <v>2.23</v>
+      </c>
+      <c r="U10" s="15">
+        <f>(O10-R10)/S10</f>
+        <v>8.0896860986547081E-3</v>
+      </c>
+      <c r="V10" s="15">
+        <f t="shared" si="0"/>
+        <v>1.6620488478249703E-4</v>
+      </c>
+      <c r="W10" s="14">
+        <f t="shared" si="1"/>
+        <v>48.672974378829025</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="15">
+        <v>14.31</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1.6000000000000014E-2</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0.1166</v>
+      </c>
+      <c r="E11" s="21">
+        <v>1.2105842409643557</v>
+      </c>
+      <c r="F11" s="42">
+        <v>5.0875790391743614E-2</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18">
+        <v>2</v>
+      </c>
+      <c r="I11" s="18">
+        <v>2</v>
+      </c>
+      <c r="J11" s="16">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K11" s="16">
+        <v>999</v>
+      </c>
+      <c r="L11" s="16">
+        <v>26.9</v>
+      </c>
+      <c r="M11" s="15">
+        <v>99.81</v>
+      </c>
+      <c r="N11" s="15">
+        <v>7.8939399999999997</v>
+      </c>
+      <c r="O11" s="14">
+        <v>0.24668999999999999</v>
+      </c>
+      <c r="P11" s="15">
+        <v>88.14</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>6.9709700000000003</v>
+      </c>
+      <c r="R11" s="14">
+        <v>0.21784999999999999</v>
+      </c>
+      <c r="S11" s="14">
+        <v>2.23</v>
+      </c>
+      <c r="U11" s="15">
+        <f>(O11-R11)/S11</f>
+        <v>1.293273542600897E-2</v>
+      </c>
+      <c r="V11" s="15">
+        <f t="shared" si="0"/>
+        <v>1.6288078708684792E-3</v>
+      </c>
+      <c r="W11" s="14">
+        <f t="shared" si="1"/>
+        <v>7.9400005717759976</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="15">
+        <v>11.61</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1.319999999999999E-2</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0.11890000000000001</v>
+      </c>
+      <c r="E12" s="21">
+        <v>1.2344647140053784</v>
+      </c>
+      <c r="F12" s="42">
+        <v>7.4756263432766312E-2</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18">
+        <v>2</v>
+      </c>
+      <c r="I12" s="18">
+        <v>3</v>
+      </c>
+      <c r="J12" s="16">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K12" s="16">
+        <v>999</v>
+      </c>
+      <c r="L12" s="16">
+        <v>26.9</v>
+      </c>
+      <c r="M12" s="15">
+        <v>98.64</v>
+      </c>
+      <c r="N12" s="15">
+        <v>7.8014099999999997</v>
+      </c>
+      <c r="O12" s="14">
+        <v>0.24379999999999999</v>
+      </c>
+      <c r="P12" s="15">
+        <v>86.76</v>
+      </c>
+      <c r="Q12" s="15">
+        <v>6.8618199999999998</v>
+      </c>
+      <c r="R12" s="14">
+        <v>0.21443999999999999</v>
+      </c>
+      <c r="S12" s="14">
+        <v>2.23</v>
+      </c>
+      <c r="U12" s="15">
+        <f>(O12-R12)/S12</f>
+        <v>1.3165919282511209E-2</v>
+      </c>
+      <c r="V12" s="15">
+        <f t="shared" si="0"/>
+        <v>2.3933503408679756E-3</v>
+      </c>
+      <c r="W12" s="14">
+        <f>U12/V12</f>
+        <v>5.5010413885902052</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="15">
+        <v>7.42</v>
+      </c>
+      <c r="C13" s="15">
+        <v>2.3999999999999577E-3</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0.112</v>
+      </c>
+      <c r="E13" s="21">
+        <v>1.1628232948823107</v>
+      </c>
+      <c r="F13" s="42">
+        <v>3.1148443096986611E-3</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18">
+        <v>2</v>
+      </c>
+      <c r="I13" s="18">
+        <v>5</v>
+      </c>
+      <c r="J13" s="16">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K13" s="16">
+        <v>999</v>
+      </c>
+      <c r="L13" s="16">
+        <v>26.9</v>
+      </c>
+      <c r="M13" s="15">
+        <v>99.34</v>
+      </c>
+      <c r="N13" s="15">
+        <v>7.85677</v>
+      </c>
+      <c r="O13" s="14">
+        <v>0.24553</v>
+      </c>
+      <c r="P13" s="15">
+        <v>88.9</v>
+      </c>
+      <c r="Q13" s="15">
+        <v>7.0310699999999997</v>
+      </c>
+      <c r="R13" s="14">
+        <v>0.21973000000000001</v>
+      </c>
+      <c r="S13" s="14">
+        <v>2.23</v>
+      </c>
+      <c r="U13" s="15">
+        <f>(O13-R13)/S13</f>
+        <v>1.1569506726457394E-2</v>
+      </c>
+      <c r="V13" s="15">
+        <f t="shared" si="0"/>
+        <v>9.9722930869501061E-5</v>
+      </c>
+      <c r="W13" s="14">
+        <f t="shared" si="1"/>
+        <v>116.01651320895719</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="15">
+        <v>13.49</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1.4300000000000035E-2</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0.11550000000000001</v>
+      </c>
+      <c r="E14" s="21">
+        <v>1.1991631451621276</v>
+      </c>
+      <c r="F14" s="42">
+        <v>3.945469458951556E-2</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="24">
+        <v>2</v>
+      </c>
+      <c r="I14" s="24">
+        <v>6</v>
+      </c>
+      <c r="J14" s="16">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K14" s="16">
+        <v>999</v>
+      </c>
+      <c r="L14" s="16">
+        <v>26.9</v>
+      </c>
+      <c r="M14" s="15">
+        <v>99.43</v>
+      </c>
+      <c r="N14" s="15">
+        <v>7.8638899999999996</v>
+      </c>
+      <c r="O14" s="14">
+        <v>0.24576000000000001</v>
+      </c>
+      <c r="P14" s="15">
+        <v>86.68</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>6.8554899999999996</v>
+      </c>
+      <c r="R14" s="14">
+        <v>0.21424000000000001</v>
+      </c>
+      <c r="S14" s="14">
+        <v>2.23</v>
+      </c>
+      <c r="U14" s="15">
+        <f>(O14-R14)/S14</f>
+        <v>1.4134529147982059E-2</v>
+      </c>
+      <c r="V14" s="15">
+        <f t="shared" si="0"/>
+        <v>1.2631571243469873E-3</v>
+      </c>
+      <c r="W14" s="14">
+        <f t="shared" si="1"/>
+        <v>11.189842400080803</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="15">
+        <v>10.1</v>
+      </c>
+      <c r="C15" s="15">
+        <v>7.3999999999999622E-3</v>
+      </c>
+      <c r="D15" s="25">
+        <v>0.1132</v>
+      </c>
+      <c r="E15" s="21">
+        <v>1.1752826721211052</v>
+      </c>
+      <c r="F15" s="42">
+        <v>1.5574221548493083E-2</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18">
+        <v>2</v>
+      </c>
+      <c r="I15" s="18">
+        <v>7</v>
+      </c>
+      <c r="J15" s="16">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K15" s="16">
+        <v>999</v>
+      </c>
+      <c r="L15" s="16">
+        <v>26.9</v>
+      </c>
+      <c r="M15" s="15">
+        <v>99.43</v>
+      </c>
+      <c r="N15" s="15">
+        <v>7.8638899999999996</v>
+      </c>
+      <c r="O15" s="14">
+        <v>0.24576000000000001</v>
+      </c>
+      <c r="P15" s="15">
+        <v>82.24</v>
+      </c>
+      <c r="Q15" s="15">
+        <v>6.50434</v>
+      </c>
+      <c r="R15" s="14">
+        <v>0.20327000000000001</v>
+      </c>
+      <c r="S15" s="14">
+        <v>2.23</v>
+      </c>
+      <c r="U15" s="15">
+        <f>(O15-R15)/S15</f>
+        <v>1.9053811659192826E-2</v>
+      </c>
+      <c r="V15" s="15">
+        <f>((F15)*(1/14.00672))/S15</f>
+        <v>4.9861465434749826E-4</v>
+      </c>
+      <c r="W15" s="14">
+        <f t="shared" si="1"/>
+        <v>38.213501133710565</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="28">
-        <v>0.1157</v>
-      </c>
-      <c r="C6" s="34">
-        <v>1.2012397080352599</v>
-      </c>
-      <c r="D6" s="43">
-        <v>9.4483610727523759E-2</v>
-      </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31">
+      <c r="B16" s="15">
+        <v>12.53</v>
+      </c>
+      <c r="C16" s="15">
+        <v>1.4299999999999979E-2</v>
+      </c>
+      <c r="D16" s="25">
+        <v>0.11550000000000001</v>
+      </c>
+      <c r="E16" s="21">
+        <v>1.1991631451621276</v>
+      </c>
+      <c r="F16" s="42">
+        <v>3.0110161660419577E-2</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18">
+        <v>3</v>
+      </c>
+      <c r="I16" s="18">
         <v>1</v>
       </c>
-      <c r="G6" s="31">
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="15">
+        <v>11.4</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="D17" s="25">
+        <v>0.11840000000000001</v>
+      </c>
+      <c r="E17" s="21">
+        <v>1.2292733068225474</v>
+      </c>
+      <c r="F17" s="42">
+        <v>6.0220323320839375E-2</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18">
         <v>3</v>
       </c>
-      <c r="H6" s="29">
-        <v>19.579999999999998</v>
-      </c>
-      <c r="I6" s="29">
-        <v>1020</v>
-      </c>
-      <c r="J6" s="29">
-        <v>26.5</v>
-      </c>
-      <c r="K6" s="28">
-        <v>98.17</v>
-      </c>
-      <c r="L6" s="28">
-        <v>7.76424</v>
-      </c>
-      <c r="M6" s="26">
-        <v>0.24263999999999999</v>
-      </c>
-      <c r="N6" s="28">
-        <v>81.27</v>
-      </c>
-      <c r="O6" s="28">
-        <v>6.4276200000000001</v>
-      </c>
-      <c r="P6" s="26">
-        <v>0.20086999999999999</v>
-      </c>
-      <c r="Q6" s="43">
-        <v>2.72</v>
-      </c>
-      <c r="R6" s="33"/>
-      <c r="S6" s="28">
-        <f t="shared" si="0"/>
-        <v>1.5356617647058823E-2</v>
-      </c>
-      <c r="T6" s="28">
-        <f t="shared" si="1"/>
-        <v>2.4799968580082547E-3</v>
-      </c>
-      <c r="U6" s="26">
-        <f t="shared" si="2"/>
-        <v>6.1921923801920027</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="28">
-        <v>0.11360000000000001</v>
-      </c>
-      <c r="C7" s="34">
-        <v>1.17943579786737</v>
-      </c>
-      <c r="D7" s="43">
-        <v>5.3990634701442275E-2</v>
-      </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31">
-        <v>1</v>
-      </c>
-      <c r="G7" s="31">
+      <c r="I17" s="18">
+        <v>2</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="40">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="C18" s="40">
+        <v>12.998266897746971</v>
+      </c>
+      <c r="D18" s="25">
+        <v>0.1172</v>
+      </c>
+      <c r="E18" s="21">
+        <v>1.216813929583753</v>
+      </c>
+      <c r="F18" s="42">
+        <v>5.9182041884273229E-2</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18">
+        <v>3</v>
+      </c>
+      <c r="I18" s="18">
+        <v>3</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="40">
+        <v>9.51</v>
+      </c>
+      <c r="C19" s="40">
+        <v>11.187607573149755</v>
+      </c>
+      <c r="D19" s="25">
+        <v>0.1162</v>
+      </c>
+      <c r="E19" s="21">
+        <v>1.2064311152180911</v>
+      </c>
+      <c r="F19" s="42">
+        <v>4.8799227518611321E-2</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="18">
+        <v>3</v>
+      </c>
+      <c r="I19" s="18">
         <v>5</v>
       </c>
-      <c r="H7" s="29">
-        <v>19.579999999999998</v>
-      </c>
-      <c r="I7" s="29">
-        <v>1020</v>
-      </c>
-      <c r="J7" s="29">
-        <v>26.5</v>
-      </c>
-      <c r="K7" s="28">
-        <v>103.65</v>
-      </c>
-      <c r="L7" s="28">
-        <v>8.1976499999999994</v>
-      </c>
-      <c r="M7" s="26">
-        <v>0.25618999999999997</v>
-      </c>
-      <c r="N7" s="28">
-        <v>83.89</v>
-      </c>
-      <c r="O7" s="28">
-        <v>6.63483</v>
-      </c>
-      <c r="P7" s="26">
-        <v>0.20735000000000001</v>
-      </c>
-      <c r="Q7" s="43">
-        <v>2.72</v>
-      </c>
-      <c r="R7" s="33"/>
-      <c r="S7" s="28">
-        <f t="shared" si="0"/>
-        <v>1.7955882352941162E-2</v>
-      </c>
-      <c r="T7" s="28">
-        <f t="shared" si="1"/>
-        <v>1.4171410617190058E-3</v>
-      </c>
-      <c r="U7" s="26">
-        <f t="shared" si="2"/>
-        <v>12.670497551711968</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="28">
-        <v>0.1086</v>
-      </c>
-      <c r="C8" s="34">
-        <v>1.1275217260390602</v>
-      </c>
-      <c r="D8" s="44">
-        <v>2.07656287313251E-3</v>
-      </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37">
-        <v>1</v>
-      </c>
-      <c r="G8" s="37">
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="40">
+        <v>8.89</v>
+      </c>
+      <c r="C20" s="40">
+        <v>12.649164677804361</v>
+      </c>
+      <c r="D20" s="25">
+        <v>0.1145</v>
+      </c>
+      <c r="E20" s="21">
+        <v>1.1887803307964657</v>
+      </c>
+      <c r="F20" s="42">
+        <v>3.1148443096985945E-2</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="18">
+        <v>3</v>
+      </c>
+      <c r="I20" s="24">
         <v>6</v>
       </c>
-      <c r="H8" s="29">
-        <v>19.579999999999998</v>
-      </c>
-      <c r="I8" s="29">
-        <v>1020</v>
-      </c>
-      <c r="J8" s="29">
-        <v>26.5</v>
-      </c>
-      <c r="K8" s="28">
-        <v>100.5</v>
-      </c>
-      <c r="L8" s="28">
-        <v>7.9485099999999997</v>
-      </c>
-      <c r="M8" s="26">
-        <v>0.24840000000000001</v>
-      </c>
-      <c r="N8" s="28">
-        <v>95.42</v>
-      </c>
-      <c r="O8" s="28">
-        <v>7.5467399999999998</v>
-      </c>
-      <c r="P8" s="26">
-        <v>0.23583999999999999</v>
-      </c>
-      <c r="Q8" s="43">
-        <v>2.72</v>
-      </c>
-      <c r="R8" s="33"/>
-      <c r="S8" s="28">
-        <f t="shared" si="0"/>
-        <v>4.6176470588235345E-3</v>
-      </c>
-      <c r="T8" s="38">
-        <f t="shared" si="1"/>
-        <v>5.4505425450734011E-5</v>
-      </c>
-      <c r="U8" s="27">
-        <f t="shared" si="2"/>
-        <v>84.719035227003261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="28">
-        <v>0.11219999999999999</v>
-      </c>
-      <c r="C9" s="34">
-        <v>1.164899857755443</v>
-      </c>
-      <c r="D9" s="43">
-        <v>5.1914071828309538E-3</v>
-      </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31">
-        <v>1</v>
-      </c>
-      <c r="G9" s="31">
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="40">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="C21" s="40">
+        <v>10.771704180064287</v>
+      </c>
+      <c r="D21" s="15">
+        <v>0.1164</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1.2085076780912234</v>
+      </c>
+      <c r="F21" s="42">
+        <v>5.0875790391743614E-2</v>
+      </c>
+      <c r="H21" s="18">
+        <v>3</v>
+      </c>
+      <c r="I21" s="18">
         <v>7</v>
       </c>
-      <c r="H9" s="29">
-        <v>19.579999999999998</v>
-      </c>
-      <c r="I9" s="29">
-        <v>1020</v>
-      </c>
-      <c r="J9" s="29">
-        <v>26.5</v>
-      </c>
-      <c r="K9" s="28">
-        <v>101.1</v>
-      </c>
-      <c r="L9" s="28">
-        <v>7.9959699999999998</v>
-      </c>
-      <c r="M9" s="26">
-        <v>0.24987999999999999</v>
-      </c>
-      <c r="N9" s="28">
-        <v>94.62</v>
-      </c>
-      <c r="O9" s="28">
-        <v>7.4834699999999996</v>
-      </c>
-      <c r="P9" s="26">
-        <v>0.23386999999999999</v>
-      </c>
-      <c r="Q9" s="43">
-        <v>2.72</v>
-      </c>
-      <c r="R9" s="33"/>
-      <c r="S9" s="28">
-        <f t="shared" si="0"/>
-        <v>5.886029411764704E-3</v>
-      </c>
-      <c r="T9" s="28">
-        <f t="shared" si="1"/>
-        <v>1.362635636268266E-4</v>
-      </c>
-      <c r="U9" s="26">
-        <f t="shared" si="2"/>
-        <v>43.195915731987391</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="28">
-        <v>0.1166</v>
-      </c>
-      <c r="C10" s="34">
-        <v>1.2105842409643557</v>
-      </c>
-      <c r="D10" s="43">
-        <v>5.0875790391743614E-2</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31">
-        <v>2</v>
-      </c>
-      <c r="G10" s="31">
-        <v>1</v>
-      </c>
-      <c r="H10" s="29">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I10" s="29">
-        <v>999</v>
-      </c>
-      <c r="J10" s="29">
-        <v>26.9</v>
-      </c>
-      <c r="K10" s="28">
-        <v>100.87</v>
-      </c>
-      <c r="L10" s="28">
-        <v>7.9777800000000001</v>
-      </c>
-      <c r="M10" s="26">
-        <v>0.24931</v>
-      </c>
-      <c r="N10" s="28">
-        <v>93.57</v>
-      </c>
-      <c r="O10" s="28">
-        <v>7.4004200000000004</v>
-      </c>
-      <c r="P10" s="26">
-        <v>0.23127</v>
-      </c>
-      <c r="Q10" s="26">
-        <v>2.23</v>
-      </c>
-      <c r="R10" s="33"/>
-      <c r="S10" s="28">
-        <f t="shared" si="0"/>
-        <v>8.0896860986547081E-3</v>
-      </c>
-      <c r="T10" s="28">
-        <f t="shared" ref="T10:T15" si="3">((D10)*(1/14.00672))/Q10</f>
-        <v>1.6288078708684792E-3</v>
-      </c>
-      <c r="U10" s="26">
-        <f t="shared" si="2"/>
-        <v>4.9666300386559978</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="28">
-        <v>0.11890000000000001</v>
-      </c>
-      <c r="C11" s="34">
-        <v>1.2344647140053784</v>
-      </c>
-      <c r="D11" s="43">
-        <v>7.4756263432766312E-2</v>
-      </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31">
-        <v>2</v>
-      </c>
-      <c r="G11" s="31">
-        <v>2</v>
-      </c>
-      <c r="H11" s="29">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I11" s="29">
-        <v>999</v>
-      </c>
-      <c r="J11" s="29">
-        <v>26.9</v>
-      </c>
-      <c r="K11" s="28">
-        <v>99.81</v>
-      </c>
-      <c r="L11" s="28">
-        <v>7.8939399999999997</v>
-      </c>
-      <c r="M11" s="26">
-        <v>0.24668999999999999</v>
-      </c>
-      <c r="N11" s="28">
-        <v>88.14</v>
-      </c>
-      <c r="O11" s="28">
-        <v>6.9709700000000003</v>
-      </c>
-      <c r="P11" s="26">
-        <v>0.21784999999999999</v>
-      </c>
-      <c r="Q11" s="26">
-        <v>2.23</v>
-      </c>
-      <c r="R11" s="33"/>
-      <c r="S11" s="28">
-        <f t="shared" si="0"/>
-        <v>1.293273542600897E-2</v>
-      </c>
-      <c r="T11" s="28">
-        <f t="shared" si="3"/>
-        <v>2.3933503408679756E-3</v>
-      </c>
-      <c r="U11" s="26">
-        <f t="shared" si="2"/>
-        <v>5.4036115002364289</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="28">
-        <v>0.112</v>
-      </c>
-      <c r="C12" s="34">
-        <v>1.1628232948823107</v>
-      </c>
-      <c r="D12" s="43">
-        <v>3.1148443096986611E-3</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31">
-        <v>2</v>
-      </c>
-      <c r="G12" s="31">
-        <v>3</v>
-      </c>
-      <c r="H12" s="29">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I12" s="29">
-        <v>999</v>
-      </c>
-      <c r="J12" s="29">
-        <v>26.9</v>
-      </c>
-      <c r="K12" s="28">
-        <v>98.64</v>
-      </c>
-      <c r="L12" s="28">
-        <v>7.8014099999999997</v>
-      </c>
-      <c r="M12" s="26">
-        <v>0.24379999999999999</v>
-      </c>
-      <c r="N12" s="28">
-        <v>86.76</v>
-      </c>
-      <c r="O12" s="28">
-        <v>6.8618199999999998</v>
-      </c>
-      <c r="P12" s="26">
-        <v>0.21443999999999999</v>
-      </c>
-      <c r="Q12" s="26">
-        <v>2.23</v>
-      </c>
-      <c r="R12" s="33"/>
-      <c r="S12" s="28">
-        <f t="shared" si="0"/>
-        <v>1.3165919282511209E-2</v>
-      </c>
-      <c r="T12" s="28">
-        <f t="shared" si="3"/>
-        <v>9.9722930869501061E-5</v>
-      </c>
-      <c r="U12" s="26">
-        <f>S12/T12</f>
-        <v>132.02499332616216</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="28">
-        <v>0.11550000000000001</v>
-      </c>
-      <c r="C13" s="34">
-        <v>1.1991631451621276</v>
-      </c>
-      <c r="D13" s="43">
-        <v>3.945469458951556E-2</v>
-      </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31">
-        <v>2</v>
-      </c>
-      <c r="G13" s="31">
-        <v>5</v>
-      </c>
-      <c r="H13" s="29">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I13" s="29">
-        <v>999</v>
-      </c>
-      <c r="J13" s="29">
-        <v>26.9</v>
-      </c>
-      <c r="K13" s="28">
-        <v>99.34</v>
-      </c>
-      <c r="L13" s="28">
-        <v>7.85677</v>
-      </c>
-      <c r="M13" s="26">
-        <v>0.24553</v>
-      </c>
-      <c r="N13" s="28">
-        <v>88.9</v>
-      </c>
-      <c r="O13" s="28">
-        <v>7.0310699999999997</v>
-      </c>
-      <c r="P13" s="26">
-        <v>0.21973000000000001</v>
-      </c>
-      <c r="Q13" s="26">
-        <v>2.23</v>
-      </c>
-      <c r="R13" s="33"/>
-      <c r="S13" s="28">
-        <f t="shared" si="0"/>
-        <v>1.1569506726457394E-2</v>
-      </c>
-      <c r="T13" s="28">
-        <f t="shared" si="3"/>
-        <v>1.2631571243469873E-3</v>
-      </c>
-      <c r="U13" s="26">
-        <f t="shared" si="2"/>
-        <v>9.1591984112336515</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="28">
-        <v>0.1132</v>
-      </c>
-      <c r="C14" s="34">
-        <v>1.1752826721211052</v>
-      </c>
-      <c r="D14" s="43">
-        <v>1.5574221548493083E-2</v>
-      </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="37">
-        <v>2</v>
-      </c>
-      <c r="G14" s="37">
-        <v>6</v>
-      </c>
-      <c r="H14" s="29">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I14" s="29">
-        <v>999</v>
-      </c>
-      <c r="J14" s="29">
-        <v>26.9</v>
-      </c>
-      <c r="K14" s="28">
-        <v>99.43</v>
-      </c>
-      <c r="L14" s="28">
-        <v>7.8638899999999996</v>
-      </c>
-      <c r="M14" s="26">
-        <v>0.24576000000000001</v>
-      </c>
-      <c r="N14" s="28">
-        <v>86.68</v>
-      </c>
-      <c r="O14" s="28">
-        <v>6.8554899999999996</v>
-      </c>
-      <c r="P14" s="26">
-        <v>0.21424000000000001</v>
-      </c>
-      <c r="Q14" s="26">
-        <v>2.23</v>
-      </c>
-      <c r="R14" s="33"/>
-      <c r="S14" s="28">
-        <f t="shared" si="0"/>
-        <v>1.4134529147982059E-2</v>
-      </c>
-      <c r="T14" s="28">
-        <f t="shared" si="3"/>
-        <v>4.9861465434749826E-4</v>
-      </c>
-      <c r="U14" s="26">
-        <f t="shared" si="2"/>
-        <v>28.347600746871183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="39">
-        <v>0.11550000000000001</v>
-      </c>
-      <c r="C15" s="34">
-        <v>1.1991631451621276</v>
-      </c>
-      <c r="D15" s="43">
-        <v>3.0110161660419577E-2</v>
-      </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31">
-        <v>2</v>
-      </c>
-      <c r="G15" s="31">
-        <v>7</v>
-      </c>
-      <c r="H15" s="29">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I15" s="29">
-        <v>999</v>
-      </c>
-      <c r="J15" s="29">
-        <v>26.9</v>
-      </c>
-      <c r="K15" s="28">
-        <v>99.43</v>
-      </c>
-      <c r="L15" s="28">
-        <v>7.8638899999999996</v>
-      </c>
-      <c r="M15" s="26">
-        <v>0.24576000000000001</v>
-      </c>
-      <c r="N15" s="28">
-        <v>82.24</v>
-      </c>
-      <c r="O15" s="28">
-        <v>6.50434</v>
-      </c>
-      <c r="P15" s="26">
-        <v>0.20327000000000001</v>
-      </c>
-      <c r="Q15" s="26">
-        <v>2.23</v>
-      </c>
-      <c r="R15" s="33"/>
-      <c r="S15" s="28">
-        <f t="shared" si="0"/>
-        <v>1.9053811659192826E-2</v>
-      </c>
-      <c r="T15" s="28">
-        <f t="shared" si="3"/>
-        <v>9.6398833173848427E-4</v>
-      </c>
-      <c r="U15" s="26">
-        <f t="shared" si="2"/>
-        <v>19.76560403467813</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="39">
-        <v>0.11840000000000001</v>
-      </c>
-      <c r="C16" s="34">
-        <v>1.2292733068225474</v>
-      </c>
-      <c r="D16" s="29">
-        <v>6.0220323320839375E-2</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="39">
-        <v>0.1172</v>
-      </c>
-      <c r="C17" s="34">
-        <v>1.216813929583753</v>
-      </c>
-      <c r="D17" s="29">
-        <v>5.9182041884273229E-2</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="39">
-        <v>0.1162</v>
-      </c>
-      <c r="C18" s="34">
-        <v>1.2064311152180911</v>
-      </c>
-      <c r="D18" s="29">
-        <v>4.8799227518611321E-2</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="39">
-        <v>0.1145</v>
-      </c>
-      <c r="C19" s="34">
-        <v>1.1887803307964657</v>
-      </c>
-      <c r="D19" s="29">
-        <v>3.1148443096985945E-2</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="39">
-        <v>0.1164</v>
-      </c>
-      <c r="C20" s="34">
-        <v>1.2085076780912234</v>
-      </c>
-      <c r="D20" s="29">
-        <v>5.0875790391743614E-2</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="K21" s="13" t="s">
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W22" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="X22" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="M23" s="15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="K22" s="13" t="s">
+      <c r="W23" s="14">
+        <f>AVERAGE(W4:W7,W10:W12,W14:W15)</f>
+        <v>15.996206164709292</v>
+      </c>
+      <c r="X23" s="12">
+        <f>_xlfn.STDEV.S(W4:W7,W9:W11,W13:W15)</f>
+        <v>36.73462680883641</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="M24" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="U22" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="V22" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U23" s="26">
-        <f>AVERAGE(U4:U7,U9:U11,U13:U15)</f>
-        <v>14.328705607305977</v>
-      </c>
-      <c r="V23" s="13">
-        <f>_xlfn.STDEV.S(U4:U7,U9:U11,U13:U15)</f>
-        <v>12.637315259991174</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="K24" s="13" t="s">
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="M26" s="15" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>